<commit_message>
Updated source file and modelling to include plot size. Issues arise with plot size data being incomplete.
</commit_message>
<xml_diff>
--- a/Analysis/Comp_comb_coupe.xlsx
+++ b/Analysis/Comp_comb_coupe.xlsx
@@ -31650,7 +31650,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -31753,7 +31753,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -31856,7 +31856,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -31959,7 +31959,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -32062,7 +32062,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -32165,7 +32165,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Quercus sp. and Carya sp.</t>
+          <t>Various</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">

</xml_diff>